<commit_message>
Actualizar menú desde Excel
</commit_message>
<xml_diff>
--- a/public/restaurant_products.xlsx
+++ b/public/restaurant_products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renzo\01_SISTEMAS\qumara\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7D8B61-1BB9-47BC-B294-779DEDF2B6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C54062-5564-41AB-879A-F6D3D4DEC310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -1073,7 +1073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -1877,7 +1877,7 @@
         <v>128</v>
       </c>
       <c r="D31">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E31" t="s">
         <v>96</v>
@@ -2086,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BBF831B-95AE-42BD-BA3B-F71C2ECBD330}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2120,7 +2120,7 @@
         <v>82</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>
@@ -2137,7 +2137,7 @@
         <v>84</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>88</v>

</xml_diff>